<commit_message>
Second major update [v1.1] - Automatic detection of week and day numbers - Added saving the last message to avoid an error on a new request - Fixed a problem when receiving a random message about the processing of an AI request. - Optimized schedule processing structure for the selected day - Improved project structure
</commit_message>
<xml_diff>
--- a/Schedules/Xlsx/ИСб-21-2-о (15 нед.).xlsx
+++ b/Schedules/Xlsx/ИСб-21-2-о (15 нед.).xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1476,6 +1476,9 @@
         </is>
       </c>
     </row>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>